<commit_message>
Updated level 1 classifications for tabula muris.
</commit_message>
<xml_diff>
--- a/CTD_code/tm_level1classifications_full.xlsx
+++ b/CTD_code/tm_level1classifications_full.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\rare_disease_ewce\CTD_code\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchap\OneDrive\Documents\Imperial\Year 3\Project\Tabula Muris Levels 1 and 2 Generation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293B96FA-8CFB-41CC-BF3B-DD5956440BF3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770440D5-C1C2-4BCC-AD71-2C24A8D3AAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E29340F-2985-41E3-8BEE-8ADE82AB86CA}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E29340F-2985-41E3-8BEE-8ADE82AB86CA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="78">
   <si>
     <t>Bladder cells</t>
   </si>
@@ -59,24 +59,9 @@
     <t>Endothelial cells</t>
   </si>
   <si>
-    <t>Pancreatic islet cells</t>
-  </si>
-  <si>
-    <t>pancreatic A cell_Pancreas, type B pancreatic cell_Pancreas, pancreatic acinar cell_Pancreas, pancreatic PP cell_Pancreas, pancreatic D cell_Pancreas</t>
-  </si>
-  <si>
-    <t>Pancreatic non-islet cells</t>
-  </si>
-  <si>
-    <t>pancreatic ductal cell_Pancreas, pancreatic stellate cell_Pancreas</t>
-  </si>
-  <si>
     <t>Epidermal cells</t>
   </si>
   <si>
-    <t>B cell_Fat, B cell_Lung, B cell_Limb_Muscle, B cell_Marrow, B cell_Spleen, B cell_Liver, lymphocyte_Diaphragm, leukocyte_Thymus, leukocyte_Kidney, naive B cell_Marrow</t>
-  </si>
-  <si>
     <t>neuron_Brain_Non-Myeloid</t>
   </si>
   <si>
@@ -107,9 +92,6 @@
     <t>Unclassified leukocytes</t>
   </si>
   <si>
-    <t>leukocyte_Skin, leukocyte_Lung, leukocyte_Heart</t>
-  </si>
-  <si>
     <t>Immature natural killer T cells</t>
   </si>
   <si>
@@ -188,9 +170,6 @@
     <t>epithelial cell_Trachea, epithelial cell of lung_Lung, epithelial cell of proximal tubule_Kidney, epithelial cell of large intestine_Large_Intestine, kidney collecting duct epithelial cell_Kidney, ciliated columnar cell of tracheobronchial tree_Lung, luminal epithelial cell of mammary gland_Mammary_Gland</t>
   </si>
   <si>
-    <t>T cell_Fat, T cell_Lung, T cell_Limb_Muscle, T cell_Spleen, regulatory T cell_Marrow</t>
-  </si>
-  <si>
     <t>endothelial cell_Brain_Non-Myeloid, endothelial cell_Fat, endothelial cell_Trachea, endothelial cell_Kidney, endothelial cell_Pancreas, endothelial cell_Limb_Muscle, endothelial cell_Mammary_Gland, endothelial cell of hepatic sinusoid_Liver, endothelial cell_Heart, endothelial cell_Aorta, lung endothelial cell_Lung, endothelial cell_Diaphragm, endocardial cell_Heart</t>
   </si>
   <si>
@@ -209,9 +188,6 @@
     <t>immature natural killer cell_Marrow, pre-natural killer cell_Marrow</t>
   </si>
   <si>
-    <t>myeloid cell_Fat, blood cell_Trachea, myeloid cell_Lung, leukocyte_Pancreas, granulocytopoietic cell_Marrow, professional antigen presenting cell_Aorta</t>
-  </si>
-  <si>
     <t>Unclassified Cells</t>
   </si>
   <si>
@@ -249,6 +225,48 @@
   </si>
   <si>
     <t>NA_Fat, NA_Heart, NA_Lung</t>
+  </si>
+  <si>
+    <t>B cell_Fat, B cell_Lung, B cell_Limb_Muscle, B cell_Marrow, B cell_Spleen, B cell_Liver, naive B cell_Marrow</t>
+  </si>
+  <si>
+    <t>Pancreatic islets</t>
+  </si>
+  <si>
+    <t>pancreatic A cell_Pancreas, type B pancreatic cell_Pancreas, pancreatic PP cell_Pancreas, pancreatic D cell_Pancreas</t>
+  </si>
+  <si>
+    <t>Pancreatic acinar cells</t>
+  </si>
+  <si>
+    <t>pancreatic acinar cell_Pancreas</t>
+  </si>
+  <si>
+    <t>Pancreatic ductal cells</t>
+  </si>
+  <si>
+    <t>pancreatic ductal cell_Pancreas</t>
+  </si>
+  <si>
+    <t>pancreatic stellate cell_Pancreas</t>
+  </si>
+  <si>
+    <t>Pancreatic stellate cells</t>
+  </si>
+  <si>
+    <t>T cell_Fat, T cell_Lung, T cell_Limb_Muscle, T cell_Spleen</t>
+  </si>
+  <si>
+    <t>Regulatory T cells</t>
+  </si>
+  <si>
+    <t>regulatory T cell_Marrow</t>
+  </si>
+  <si>
+    <t>myeloid cell_Fat, blood cell_Trachea, myeloid cell_Lung, granulocytopoietic cell_Marrow, professional antigen presenting cell_Aorta</t>
+  </si>
+  <si>
+    <t>leukocyte_Skin, leukocyte_Lung, leukocyte_Heart, lymphocyte_Diaphragm, leukocyte_Thymus, leukocyte_Kidney, leukocyte_Pancreas</t>
   </si>
 </sst>
 </file>
@@ -600,10 +618,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1410704B-F8A4-4FC2-B6D2-01D539FDB3BA}">
-  <dimension ref="A1:B36"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -633,7 +651,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -641,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -649,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>73</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -657,250 +675,275 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>65</v>
       </c>
       <c r="B7" t="s">
-        <v>9</v>
+        <v>66</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>10</v>
+        <v>72</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>20</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>24</v>
+        <v>77</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="B21" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B24" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B25" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B27" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B31" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B32" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B33" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>54</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="B35" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="B36" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>67</v>
+      </c>
+      <c r="B37" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>74</v>
+      </c>
+      <c r="B39" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated cell type labels
</commit_message>
<xml_diff>
--- a/CTD_code/tm_level1classifications_full.xlsx
+++ b/CTD_code/tm_level1classifications_full.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jchap\OneDrive\Documents\Imperial\Year 3\Project\Tabula Muris Levels 1 and 2 Generation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitRepo\rare_disease_ewce\CTD_code\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{770440D5-C1C2-4BCC-AD71-2C24A8D3AAE3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F469058-41E4-464D-BCCF-EBB2D539D939}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8E29340F-2985-41E3-8BEE-8ADE82AB86CA}"/>
   </bookViews>
@@ -80,18 +80,12 @@
     <t>Mesenchymal cells</t>
   </si>
   <si>
-    <t>Unclassified myeloid cells</t>
-  </si>
-  <si>
     <t>Immature T cells</t>
   </si>
   <si>
     <t>mesenchymal stem cell of adipose_Fat, mesenchymal cell_Trachea, mesenchymal stem cell_Limb_Muscle, mesenchymal stem cell_Diaphragm, fibroblast_Heart, fibroblast_Aorta, stromal cell_Lung, stromal cell_Mammary_Gland, myofibroblast cell_Heart</t>
   </si>
   <si>
-    <t>Unclassified leukocytes</t>
-  </si>
-  <si>
     <t>Immature natural killer T cells</t>
   </si>
   <si>
@@ -188,12 +182,6 @@
     <t>immature natural killer cell_Marrow, pre-natural killer cell_Marrow</t>
   </si>
   <si>
-    <t>Unclassified Cells</t>
-  </si>
-  <si>
-    <t>Progenitor immune cells (Marrow)</t>
-  </si>
-  <si>
     <t>macrophage_Kidney, macrophage_Limb_Muscle, macrophage_Spleen, macrophage_Diaphragm, macrophage_Marrow, macrophage_Brain_Myeloid</t>
   </si>
   <si>
@@ -209,9 +197,6 @@
     <t>Neurons</t>
   </si>
   <si>
-    <t>Oligodendrocyte and related cells</t>
-  </si>
-  <si>
     <t>oligodendrocyte precursor cell_Brain_Non-Myeloid, oligodendrocyte_Brain_Non-Myeloid</t>
   </si>
   <si>
@@ -267,6 +252,21 @@
   </si>
   <si>
     <t>leukocyte_Skin, leukocyte_Lung, leukocyte_Heart, lymphocyte_Diaphragm, leukocyte_Thymus, leukocyte_Kidney, leukocyte_Pancreas</t>
+  </si>
+  <si>
+    <t>Myeloid cells (other)</t>
+  </si>
+  <si>
+    <t>Leukocytes (other)</t>
+  </si>
+  <si>
+    <t>Progenitor immune cells</t>
+  </si>
+  <si>
+    <t>Unclassified cells</t>
+  </si>
+  <si>
+    <t>Oligodendrocytes</t>
   </si>
 </sst>
 </file>
@@ -621,7 +621,7 @@
   <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -651,7 +651,7 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -659,7 +659,7 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -667,7 +667,7 @@
         <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -675,23 +675,23 @@
         <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="B7" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B8" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -699,20 +699,20 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
         <v>9</v>
@@ -720,10 +720,10 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B12" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -739,7 +739,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -747,7 +747,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
@@ -755,191 +755,191 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>73</v>
       </c>
       <c r="B17" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>74</v>
       </c>
       <c r="B19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B27" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>52</v>
+        <v>75</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B30" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
       <c r="B32" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B33" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B34" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
+        <v>46</v>
+      </c>
+      <c r="B35" t="s">
         <v>48</v>
-      </c>
-      <c r="B35" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B36" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="B37" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="B38" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="B39" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>